<commit_message>
Add new FGT index
</commit_message>
<xml_diff>
--- a/fgt-tables/fgt_anos_estudo_rm.xlsx
+++ b/fgt-tables/fgt_anos_estudo_rm.xlsx
@@ -379,10 +379,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3497528890897569</v>
+        <v>0.3146293670956112</v>
       </c>
       <c r="C2">
-        <v>0.002897144320992446</v>
+        <v>0.003648818996706889</v>
       </c>
     </row>
     <row r="3">
@@ -390,10 +390,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3627338938425067</v>
+        <v>0.3067188829323158</v>
       </c>
       <c r="C3">
-        <v>0.004026475388649634</v>
+        <v>0.006251139570123933</v>
       </c>
     </row>
     <row r="4">
@@ -401,10 +401,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.3830005608579209</v>
+        <v>0.3566314791467504</v>
       </c>
       <c r="C4">
-        <v>0.004763933723713355</v>
+        <v>0.007518210472485615</v>
       </c>
     </row>
     <row r="5">
@@ -412,10 +412,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.3669894805932981</v>
+        <v>0.3302645193144947</v>
       </c>
       <c r="C5">
-        <v>0.00377437128130558</v>
+        <v>0.005578099084910562</v>
       </c>
     </row>
     <row r="6">
@@ -423,10 +423,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.3457317409312652</v>
+        <v>0.305696041515249</v>
       </c>
       <c r="C6">
-        <v>0.00342695240609265</v>
+        <v>0.005087245722568943</v>
       </c>
     </row>
     <row r="7">
@@ -434,10 +434,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.2932403115250044</v>
+        <v>0.2614210394248254</v>
       </c>
       <c r="C7">
-        <v>0.002590940340337727</v>
+        <v>0.003239970372751299</v>
       </c>
     </row>
     <row r="8">
@@ -445,10 +445,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3427562358057611</v>
+        <v>0.3025824831866997</v>
       </c>
       <c r="C8">
-        <v>0.003064615212491397</v>
+        <v>0.004538753918966533</v>
       </c>
     </row>
     <row r="9">
@@ -456,10 +456,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.3489256983129703</v>
+        <v>0.3021027523813148</v>
       </c>
       <c r="C9">
-        <v>0.003652419395145504</v>
+        <v>0.005217041126488467</v>
       </c>
     </row>
     <row r="10">
@@ -467,10 +467,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.351276692183507</v>
+        <v>0.3386647529303305</v>
       </c>
       <c r="C10">
-        <v>0.003413127356165392</v>
+        <v>0.005615282256397132</v>
       </c>
     </row>
     <row r="11">
@@ -478,10 +478,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.2876495764036933</v>
+        <v>0.2587795962665891</v>
       </c>
       <c r="C11">
-        <v>0.00274044799228283</v>
+        <v>0.003925219762725651</v>
       </c>
     </row>
     <row r="12">
@@ -489,10 +489,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.3338396303731312</v>
+        <v>0.3240203674843917</v>
       </c>
       <c r="C12">
-        <v>0.003724936858498021</v>
+        <v>0.007021938290808478</v>
       </c>
     </row>
     <row r="13">
@@ -500,10 +500,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.303804647630759</v>
+        <v>0.2914894387684464</v>
       </c>
       <c r="C13">
-        <v>0.003689558035724277</v>
+        <v>0.00631817727714739</v>
       </c>
     </row>
     <row r="14">
@@ -511,10 +511,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.213204537516907</v>
+        <v>0.2067006618075515</v>
       </c>
       <c r="C14">
-        <v>0.001911177890994506</v>
+        <v>0.002383590027845342</v>
       </c>
     </row>
     <row r="15">
@@ -522,10 +522,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.1285589694756284</v>
+        <v>0.1264794623308638</v>
       </c>
       <c r="C15">
-        <v>0.003246705388001534</v>
+        <v>0.005508080263651596</v>
       </c>
     </row>
     <row r="16">
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.09761841799154779</v>
+        <v>0.09151841352835277</v>
       </c>
       <c r="C16">
-        <v>0.00324847655295997</v>
+        <v>0.005697387575726859</v>
       </c>
     </row>
     <row r="17">
@@ -544,10 +544,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.09504596227426164</v>
+        <v>0.09061337401526949</v>
       </c>
       <c r="C17">
-        <v>0.003214007210961275</v>
+        <v>0.005532012816701792</v>
       </c>
     </row>
     <row r="18">
@@ -555,10 +555,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.0457461854227854</v>
+        <v>0.04156291724602371</v>
       </c>
       <c r="C18">
-        <v>0.001038686708239315</v>
+        <v>0.001320968378429379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>